<commit_message>
Estimate with new moments
1. New moments in II procedure. I added the correlation between measures
of academic achievement in t=2 and t=5 for young and old
2. Change age for moments of young children (inputs at t=1 and measures
at t=2)
3. Fix fit code accordingly
</commit_message>
<xml_diff>
--- a/model/approx timing.xlsx
+++ b/model/approx timing.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="47">
   <si>
     <t>emax</t>
   </si>
@@ -109,12 +109,72 @@
   </si>
   <si>
     <t>VERSION: afer proposal</t>
+  </si>
+  <si>
+    <t>From emax_timing code</t>
+  </si>
+  <si>
+    <t>Grid size</t>
+  </si>
+  <si>
+    <t>Sample generation (M datasets)</t>
+  </si>
+  <si>
+    <t>Aux model generation</t>
+  </si>
+  <si>
+    <t>Total (hours)</t>
+  </si>
+  <si>
+    <t>Total (secs)</t>
+  </si>
+  <si>
+    <t>N func evaluations</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Cores for M parallel</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>From sim_data</t>
+  </si>
+  <si>
+    <t>Parallel emax</t>
+  </si>
+  <si>
+    <t>V4</t>
+  </si>
+  <si>
+    <t>V5</t>
+  </si>
+  <si>
+    <t>Cores for emaxT parallel</t>
+  </si>
+  <si>
+    <t>Cores for emaxt parallel</t>
+  </si>
+  <si>
+    <t>V6</t>
+  </si>
+  <si>
+    <t>v7</t>
+  </si>
+  <si>
+    <t>Days</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -158,10 +218,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,7 +547,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.25">
@@ -826,47 +889,157 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>1536</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1800</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1800</v>
+      </c>
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>20</v>
+      </c>
+      <c r="J5">
+        <v>20</v>
+      </c>
+      <c r="K5">
+        <v>20</v>
+      </c>
+      <c r="L5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <v>50</v>
+      </c>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>20</v>
+      </c>
+      <c r="K6">
+        <v>20</v>
+      </c>
+      <c r="L6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>69</v>
+      </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>20</v>
+      </c>
+      <c r="L7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
@@ -874,8 +1047,29 @@
         <f>C7/60</f>
         <v>0.96666666666666667</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8">
+        <v>1800</v>
+      </c>
+      <c r="H8">
+        <v>1800</v>
+      </c>
+      <c r="I8">
+        <v>1800</v>
+      </c>
+      <c r="J8">
+        <v>1800</v>
+      </c>
+      <c r="K8">
+        <v>1800</v>
+      </c>
+      <c r="L8">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
@@ -883,63 +1077,254 @@
         <f>C8*200/60</f>
         <v>3.2222222222222223</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>50</v>
+      </c>
+      <c r="H9">
+        <v>50</v>
+      </c>
+      <c r="I9">
+        <v>50</v>
+      </c>
+      <c r="J9">
+        <v>50</v>
+      </c>
+      <c r="K9">
+        <v>50</v>
+      </c>
+      <c r="L9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10">
+        <v>1000</v>
+      </c>
+      <c r="H10">
+        <v>1000</v>
+      </c>
+      <c r="I10">
+        <v>1000</v>
+      </c>
+      <c r="J10">
+        <v>1000</v>
+      </c>
+      <c r="K10">
+        <v>1000</v>
+      </c>
+      <c r="L10">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="2">
+        <v>228</v>
+      </c>
+      <c r="H11" s="2">
+        <v>106</v>
+      </c>
+      <c r="I11" s="2">
+        <v>85</v>
+      </c>
+      <c r="J11" s="2">
+        <v>85</v>
+      </c>
+      <c r="K11" s="2">
+        <v>73</v>
+      </c>
+      <c r="L11" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12">
         <v>691</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="2">
+        <v>4.46E-4</v>
+      </c>
+      <c r="H12" s="2">
+        <v>4.46E-4</v>
+      </c>
+      <c r="I12" s="2">
+        <v>4.46E-4</v>
+      </c>
+      <c r="J12" s="2">
+        <v>4.46E-4</v>
+      </c>
+      <c r="K12" s="2">
+        <v>4.46E-4</v>
+      </c>
+      <c r="L12" s="2">
+        <v>4.46E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C13">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="2">
+        <f>SUM(G11:G12)</f>
+        <v>228.00044600000001</v>
+      </c>
+      <c r="H13" s="2">
+        <f>SUM(H11:H12)</f>
+        <v>106.000446</v>
+      </c>
+      <c r="I13" s="2">
+        <f>SUM(I11:I12)</f>
+        <v>85.000445999999997</v>
+      </c>
+      <c r="J13" s="2">
+        <f>SUM(J11:J12)</f>
+        <v>85.000445999999997</v>
+      </c>
+      <c r="K13" s="2">
+        <f>SUM(K11:K12)</f>
+        <v>73.000445999999997</v>
+      </c>
+      <c r="L13" s="2">
+        <f>SUM(L11:L12)</f>
+        <v>58.000445999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C14">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C15">
         <f>C14*C13</f>
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15">
+        <v>2456</v>
+      </c>
+      <c r="H15">
+        <v>2456</v>
+      </c>
+      <c r="I15">
+        <v>2456</v>
+      </c>
+      <c r="J15">
+        <v>2456</v>
+      </c>
+      <c r="K15">
+        <v>2456</v>
+      </c>
+      <c r="L15">
+        <v>2456</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C16">
         <f>C15*200/(60*60)</f>
-        <v>0.18333333333333332</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+        <v>6.1111111111111107</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="2">
+        <f>G15*G13/(60*60)</f>
+        <v>155.54697093777779</v>
+      </c>
+      <c r="H16" s="2">
+        <f>H15*H13/(60*60)</f>
+        <v>72.315859826666667</v>
+      </c>
+      <c r="I16" s="2">
+        <f>I15*I13/(60*60)</f>
+        <v>57.989193159999992</v>
+      </c>
+      <c r="J16" s="2">
+        <f>J15*J13/(60*60)</f>
+        <v>57.989193159999992</v>
+      </c>
+      <c r="K16" s="2">
+        <f>K15*K13/(60*60)</f>
+        <v>49.802526493333332</v>
+      </c>
+      <c r="L16" s="2">
+        <f>L15*L13/(60*60)</f>
+        <v>39.569193159999998</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="3">
+        <f>G16/24</f>
+        <v>6.4811237890740747</v>
+      </c>
+      <c r="H17" s="3">
+        <f>H16/24</f>
+        <v>3.0131608261111111</v>
+      </c>
+      <c r="I17" s="3">
+        <f>I16/24</f>
+        <v>2.4162163816666662</v>
+      </c>
+      <c r="J17" s="3">
+        <f>J16/24</f>
+        <v>2.4162163816666662</v>
+      </c>
+      <c r="K17" s="3">
+        <f>K16/24</f>
+        <v>2.0751052705555555</v>
+      </c>
+      <c r="L17" s="3">
+        <f>L16/24</f>
+        <v>1.6487163816666666</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="1">
         <f>C16+C9</f>
-        <v>3.4055555555555554</v>
+        <v>9.3333333333333321</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed mistake in table ses file
</commit_message>
<xml_diff>
--- a/model/approx timing.xlsx
+++ b/model/approx timing.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="48">
   <si>
     <t>emax</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>Days</t>
+  </si>
+  <si>
+    <t>I'm using this</t>
   </si>
 </sst>
 </file>
@@ -173,7 +176,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -192,7 +195,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,6 +205,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -218,11 +227,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -892,7 +906,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,6 +923,11 @@
         <v>27</v>
       </c>
     </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>38</v>
@@ -916,6 +935,7 @@
       <c r="F3" t="s">
         <v>28</v>
       </c>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
@@ -930,7 +950,7 @@
       <c r="H4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="5" t="s">
         <v>40</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -962,7 +982,7 @@
       <c r="H5" s="2">
         <v>5</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="4">
         <v>20</v>
       </c>
       <c r="J5">
@@ -994,7 +1014,7 @@
       <c r="H6" s="2">
         <v>0</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="4">
         <v>0</v>
       </c>
       <c r="J6">
@@ -1026,7 +1046,7 @@
       <c r="H7" s="2">
         <v>0</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="4">
         <v>0</v>
       </c>
       <c r="J7">
@@ -1056,7 +1076,7 @@
       <c r="H8">
         <v>1800</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="4">
         <v>1800</v>
       </c>
       <c r="J8">
@@ -1086,7 +1106,7 @@
       <c r="H9">
         <v>50</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="4">
         <v>50</v>
       </c>
       <c r="J9">
@@ -1111,7 +1131,7 @@
       <c r="H10">
         <v>1000</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="4">
         <v>1000</v>
       </c>
       <c r="J10">
@@ -1134,7 +1154,7 @@
       <c r="H11" s="2">
         <v>106</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="5">
         <v>85</v>
       </c>
       <c r="J11" s="2">
@@ -1163,7 +1183,7 @@
       <c r="H12" s="2">
         <v>4.46E-4</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="5">
         <v>4.46E-4</v>
       </c>
       <c r="J12" s="2">
@@ -1187,27 +1207,27 @@
         <v>33</v>
       </c>
       <c r="G13" s="2">
-        <f>SUM(G11:G12)</f>
+        <f t="shared" ref="G13:L13" si="0">SUM(G11:G12)</f>
         <v>228.00044600000001</v>
       </c>
       <c r="H13" s="2">
-        <f>SUM(H11:H12)</f>
+        <f t="shared" si="0"/>
         <v>106.000446</v>
       </c>
-      <c r="I13" s="2">
-        <f>SUM(I11:I12)</f>
+      <c r="I13" s="5">
+        <f t="shared" si="0"/>
         <v>85.000445999999997</v>
       </c>
       <c r="J13" s="2">
-        <f>SUM(J11:J12)</f>
+        <f t="shared" si="0"/>
         <v>85.000445999999997</v>
       </c>
       <c r="K13" s="2">
-        <f>SUM(K11:K12)</f>
+        <f t="shared" si="0"/>
         <v>73.000445999999997</v>
       </c>
       <c r="L13" s="2">
-        <f>SUM(L11:L12)</f>
+        <f t="shared" si="0"/>
         <v>58.000445999999997</v>
       </c>
     </row>
@@ -1218,6 +1238,7 @@
       <c r="C14">
         <v>1000</v>
       </c>
+      <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
@@ -1236,7 +1257,7 @@
       <c r="H15">
         <v>2456</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="4">
         <v>2456</v>
       </c>
       <c r="J15">
@@ -1261,27 +1282,27 @@
         <v>32</v>
       </c>
       <c r="G16" s="2">
-        <f>G15*G13/(60*60)</f>
+        <f t="shared" ref="G16:L16" si="1">G15*G13/(60*60)</f>
         <v>155.54697093777779</v>
       </c>
       <c r="H16" s="2">
-        <f>H15*H13/(60*60)</f>
+        <f t="shared" si="1"/>
         <v>72.315859826666667</v>
       </c>
-      <c r="I16" s="2">
-        <f>I15*I13/(60*60)</f>
+      <c r="I16" s="5">
+        <f t="shared" si="1"/>
         <v>57.989193159999992</v>
       </c>
       <c r="J16" s="2">
-        <f>J15*J13/(60*60)</f>
+        <f t="shared" si="1"/>
         <v>57.989193159999992</v>
       </c>
       <c r="K16" s="2">
-        <f>K15*K13/(60*60)</f>
+        <f t="shared" si="1"/>
         <v>49.802526493333332</v>
       </c>
       <c r="L16" s="2">
-        <f>L15*L13/(60*60)</f>
+        <f t="shared" si="1"/>
         <v>39.569193159999998</v>
       </c>
     </row>
@@ -1290,27 +1311,27 @@
         <v>46</v>
       </c>
       <c r="G17" s="3">
-        <f>G16/24</f>
+        <f t="shared" ref="G17:L17" si="2">G16/24</f>
         <v>6.4811237890740747</v>
       </c>
       <c r="H17" s="3">
-        <f>H16/24</f>
+        <f t="shared" si="2"/>
         <v>3.0131608261111111</v>
       </c>
-      <c r="I17" s="3">
-        <f>I16/24</f>
+      <c r="I17" s="6">
+        <f t="shared" si="2"/>
         <v>2.4162163816666662</v>
       </c>
       <c r="J17" s="3">
-        <f>J16/24</f>
+        <f t="shared" si="2"/>
         <v>2.4162163816666662</v>
       </c>
       <c r="K17" s="3">
-        <f>K16/24</f>
+        <f t="shared" si="2"/>
         <v>2.0751052705555555</v>
       </c>
       <c r="L17" s="3">
-        <f>L16/24</f>
+        <f t="shared" si="2"/>
         <v>1.6487163816666666</v>
       </c>
     </row>

</xml_diff>